<commit_message>
actualización manual, formularios PAC 2011 2012 y BMI 2012
</commit_message>
<xml_diff>
--- a/public_html/archivos/2011_PAC.xlsx
+++ b/public_html/archivos/2011_PAC.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="2011_PAC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -264,6 +264,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="U4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Nivel del último título de tercer nivel obtenido de acuerdo al registro de la SENESCYT:
+• TÉCNICO SUPERIOR 
+• TECNOLÓGICO SUPERIOR
+• TERCER NIVEL
+• DOCTOR EN FILOSOFÍA O JURISPRUDENCIA
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="V4" authorId="0">
       <text>
         <r>
@@ -554,6 +573,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="AU4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Código de registro del título en la SENESCYT (último título de cuarto nivel). Si no dispone del registro incluir “SIN REGISTRO”. En caso de seleccionar "NINGUNO" en la pregunta 41 poner "NO APLICA"</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AV4" authorId="0">
       <text>
         <r>
@@ -563,24 +595,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Código de registro del título en la SENESCYT (último título de cuarto nivel). Si no dispone del registro incluir “SIN REGISTRO”. En caso de seleccionar "NINGUNO" en la pregunta 41 poner "NO APLICA"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AW4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">Subárea del conocimiento (UNESCO, Anexo 3) a la que corresponde el último título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 41 poner "NO APLICA"
 </t>
         </r>
       </text>
     </comment>
+    <comment ref="AX4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Denominación completa del penúltimo título de cuarto nivel. De preferencia registrar el título que tenga relación con la asignatura impartida. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA"</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AY4" authorId="0">
       <text>
         <r>
@@ -590,25 +622,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Denominación completa del penúltimo título de cuarto nivel. De preferencia registrar el título que tenga relación con la asignatura impartida. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA"</t>
+          <t xml:space="preserve">Fecha del penúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 41 dejar en blanco.
+</t>
         </r>
       </text>
     </comment>
     <comment ref="AZ4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Fecha del penúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 41 dejar en blanco.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BA4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -622,6 +641,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="BA4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">País donde obtuvo el penúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BB4" authorId="0">
       <text>
         <r>
@@ -631,7 +664,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">País donde obtuvo el penúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA
+          <t xml:space="preserve">Código de registro del título en la SENESCYT (penúltimo título de tercer nivel). Si no dispone del registro incluir “SIN REGISTRO”. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA"
 </t>
         </r>
       </text>
@@ -645,25 +678,25 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código de registro del título en la SENESCYT (penúltimo título de tercer nivel). Si no dispone del registro incluir “SIN REGISTRO”. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA"
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BD4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">Subárea del conocimiento (UNESCO, Anexo 3) a la que corresponde el penúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 49 poner "NO APLICA"
 </t>
         </r>
       </text>
     </comment>
+    <comment ref="BE4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Denominación completa del antepenúltimo título de cuarto nivel. De preferencia registrar el título que tenga relación con la asignatura impartida. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BF4" authorId="0">
       <text>
         <r>
@@ -673,7 +706,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Denominación completa del antepenúltimo título de cuarto nivel. De preferencia registrar el título que tenga relación con la asignatura impartida. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
+          <t xml:space="preserve">Fecha del antepenúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 56 dejar en blanco.
 </t>
         </r>
       </text>
@@ -687,26 +720,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Fecha del antepenúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 56 dejar en blanco.
+          <t xml:space="preserve">Nombre de la institución de educación superior que le otorgó el antepenúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
 </t>
         </r>
       </text>
     </comment>
     <comment ref="BH4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Nombre de la institución de educación superior que le otorgó el antepenúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BI4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -720,6 +739,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="BI4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Código de registro del título en la SENESCYT (antepenúltimo título de cuarto nivel). Si no dispone del registro incluir “SIN REGISTRO”. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BJ4" authorId="0">
       <text>
         <r>
@@ -729,7 +762,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código de registro del título en la SENESCYT (antepenúltimo título de cuarto nivel). Si no dispone del registro incluir “SIN REGISTRO”. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
+          <t xml:space="preserve">Subárea del conocimiento (UNESCO, Anexo 3) a la que corresponde el antepenúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
 </t>
         </r>
       </text>
@@ -743,7 +776,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Subárea del conocimiento (UNESCO, Anexo 3) a la que corresponde el antepenúltimo título de cuarto nivel. En caso de seleccionar "NINGUNO" en la pregunta 56 poner "NO APLICA"
+          <t xml:space="preserve">Número del nombramiento, contrato o su equivalente.
 </t>
         </r>
       </text>
@@ -757,26 +790,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número del nombramiento, contrato o su equivalente.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="BM4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">Fecha de ingreso a la institución (formato: dd/mm/yyyy)
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="BN4" authorId="1">
+    <comment ref="BM4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -794,6 +813,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="BN4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El Ingreso a la institución se realizó mediante concurso público de merecimientos y oposición. 
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="BO4" authorId="0">
       <text>
         <r>
@@ -803,7 +836,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">El Ingreso a la institución se realizó mediante concurso público de merecimientos y oposición. 
+          <t xml:space="preserve">Nominación del cargo con el cuál fue emitido el nombramiento o contrato
 </t>
         </r>
       </text>
@@ -817,8 +850,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Nominación del cargo con el cuál fue emitido el nombramiento o contrato
-</t>
+          <t>Número total de horas laboradas al año.</t>
         </r>
       </text>
     </comment>
@@ -831,7 +863,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Número total de horas laboradas al año.</t>
+          <t xml:space="preserve">Remuneración anual que consta en el nombramiento o contrato, incluidos el décimo tercero y décimo cuarto; no incluir IVA, aportes patronales y pagos por horas extras
+</t>
         </r>
       </text>
     </comment>
@@ -844,7 +877,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Remuneración anual que consta en el nombramiento o contrato, incluidos el décimo tercero y décimo cuarto; no incluir IVA, aportes patronales y pagos por horas extras
+          <t xml:space="preserve">Fecha de salida del personal académico de la institución (formato: dd/mm/yyyy). En caso de seguir laborando dejar en blanco
 </t>
         </r>
       </text>
@@ -858,7 +891,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Fecha de salida del personal académico de la institución (formato: dd/mm/yyyy). En caso de seguir laborando dejar en blanco
+          <t xml:space="preserve">El profesor ejerce la docencia en tercer nivel
+• SI
+• NO
 </t>
         </r>
       </text>
@@ -872,7 +907,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">El profesor ejerce la docencia en tercer nivel, caso contrario poner "NO APLICA" </t>
+          <t xml:space="preserve">El profesor ejerce la docencia en cuarto nivel
+• SI
+• NO
+</t>
         </r>
       </text>
     </comment>
@@ -885,7 +923,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">El profesor ejerce la docencia en cuarto nivel, caso contrario poner "NO APLICA" </t>
+          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Obligatorio describir el código
+</t>
         </r>
       </text>
     </comment>
@@ -898,7 +937,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Obligatorio describir el código
+          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor. Obligatorio.
 </t>
         </r>
       </text>
@@ -912,7 +951,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor. Obligatorio.
+          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Obligatorio
 </t>
         </r>
       </text>
@@ -926,7 +965,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Obligatorio
+          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una segunda asignatura, colocar “NO APLICA”
 </t>
         </r>
       </text>
@@ -940,7 +979,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una segunda asignatura, colocar “NO APLICA”
+          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor. Si el profesor no dicta una segunda asignatura, colocar “NO APLICA”
 </t>
         </r>
       </text>
@@ -954,7 +993,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor. Si el profesor no dicta una segunda asignatura, colocar “NO APLICA”
+          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una segunda asignatura, colocar cero
 </t>
         </r>
       </text>
@@ -968,7 +1007,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una segunda asignatura, colocar cero
+          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una tercera asignatura, colocar “NO APLICA”
 </t>
         </r>
       </text>
@@ -982,7 +1021,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una tercera asignatura, colocar “NO APLICA”
+          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor. Si el profesor no dicta una tercera asignatura, colocar “NO APLICA”
 </t>
         </r>
       </text>
@@ -996,7 +1035,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor. Si el profesor no dicta una tercera asignatura, colocar “NO APLICA”
+          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una tercera asignatura, colocar cero
 </t>
         </r>
       </text>
@@ -1010,7 +1049,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una tercera asignatura, colocar cero
+          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una cuarta asignatura, colocar “NO APLICA”
 </t>
         </r>
       </text>
@@ -1024,7 +1063,16 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una cuarta asignatura, colocar “NO APLICA”
+          <t>Nombre de la asignatura que dicta clases el profesor. Si el profesor no dicta una cuarta asignatura, colocar “NO APLICA”</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -1038,8 +1086,595 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Nombre de la asignatura que dicta clases el profesor. Si el profesor no dicta una cuarta asignatura, colocar “NO APLICA”</t>
-        </r>
+          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una cuarta asignatura, colocar cero
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CG4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una quinta asignatura, colocar “NO APLICA”
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CH4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor Si el profesor no dicta una quinta asignatura, colocar “NO APLICA”
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CI4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una quinta asignatura, colocar cero.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CK4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Fecha inicio del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 dejar en blanco
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CL4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Fecha de finalización del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 dejar en blanco
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CM4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número del acta o documento de la elección o designación del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 poner cero
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CP4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Unidad académica a la cual pertenece 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CQ4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de horas de dedicación semanal a la docencia. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CR4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de horas de dedicación semanal a la docencia. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CS4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de horas de dirección o gestión administrativa
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CT4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de horas de dedicación semanal a vinculación con la sociedad. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CU4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Autoevaluación”. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CV4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Coevaluación de pares”. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CW4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Coevaluación de directivos”. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CX4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Heteroevaluación”. 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CY4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de cursos u otros eventos de capacitación y/o actualización realizados en el país. En caso de no disponer de cursos poner cero
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CZ4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de cursos u otros eventos de capacitación y/o actualización realizados en el extranjero. En caso de no disponer de cursos poner cero
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DA4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Número de cursos en metodologías de aprendizaje e investigación. En caso de no disponer de cursos poner cero </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DE4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Fecha de inicio del año sabático (formato: dd/mm/yyyy). En caso que no utilizó el periodo sabático dejar en blanco
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DF4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Fecha de fin del año sabático (formato: dd/mm/yyyy). En caso que no utilizó el periodo sabático dejar en blanco
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DG4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Nombre del primer libro publicado en el año. En caso de no tener publicación poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DH4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Año de publicación del primer libro. En caso de no tener publicación poner el número cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DI4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Participación en la publicación del primer libro
+• AUTOR 
+• COAUTOR
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DJ4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El primer libro antes de la publicación fue revisado por pares
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DK4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Número de ISBN del primer libro publicado. En caso de no tener publicación poner el número cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DL4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Nombre del segundo libro publicado en el año. En caso de no tener publicación poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DM4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Año de publicación del segundo libro. En caso de no tener publicación poner el número cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DN4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Participación en la publicación del segundo libro
+• AUTOR 
+• COAUTOR
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DO4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El segundo libro antes de la publicación fue revisado por pares
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DP4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Número de ISBN del segundo libro publicado. En caso de no tener publicación poner el número cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DQ4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombre del primer artículo publicado o aceptado por la publicación, en caso de no haber publicado poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DR4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombre de la revista donde se publicó el primer artículo. En caso de no haber publicado el artículo poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DS4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Año de publicación del primer artículo. En caso de no tener publicación poner el número cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DT4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Participación en la publicación del primer artículo
+• AUTOR 
+• COAUTOR
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DU4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Estado de publicación del primer artículo
+• PUBLICADO
+• ACEPTADO PARA PUBLICACIÓN
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DV4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La revista donde se publicó el primer artículo se encuentra indexada
+• SI
+• NO
+• NO APLICA
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DW4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base de datos en la cual esta indexada la revista de la publicación del primer artículo
+• ISI WEB OF KONWLEDGE 
+• SCIMAGO JOURNAL RANK (SCOPUS)
+• LATIN INDEX
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DX4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombre del segundo artículo publicado o aceptado para la publicación, en caso de no haber publicado poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DY4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombre del segundo artículo publicado o aceptado para la publicación, en caso de no haber publicado poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="DZ4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombre de la revista donde se publicó el segundo artículo. En caso de no haber publicado el artículo poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EA4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Año de publicación del segundo artículo. En caso de no tener publicación poner el número cero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EB4" authorId="1">
+      <text>
         <r>
           <rPr>
             <sz val="9"/>
@@ -1048,373 +1683,162 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CG4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una cuarta asignatura, colocar cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CH4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Código asignatura que dicta clases el profesor. Si el profesor no dicta una quinta asignatura, colocar “NO APLICA”
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CI4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Nombre de la asignatura que dicta clases el profesor Si el profesor no dicta una quinta asignatura, colocar “NO APLICA”
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CJ4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal impartida en la asignatura detallada en la variable anterior. Si el profesor no dicta una quinta asignatura, colocar cero.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CL4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Fecha inicio del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 dejar en blanco
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CM4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Fecha de finalización del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 dejar en blanco
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CN4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número del acta o documento de la elección o designación del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 poner cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CQ4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Unidad académica a la cual pertenece 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CR4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal a la docencia. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CS4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal a la docencia. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CT4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de horas de dirección o gestión administrativa
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CU4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal a vinculación con la sociedad. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CV4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Autoevaluación”. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CW4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Coevaluación de pares”. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CX4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Coevaluación de directivos”. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CY4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Porcentaje (%) que obtuvo el personal académico en la “Heteroevaluación”. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CZ4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de cursos u otros eventos de capacitación y/o actualización realizados en el país. En caso de no disponer de cursos poner cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DA4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de cursos u otros eventos de capacitación y/o actualización realizados en el extranjero. En caso de no disponer de cursos poner cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DB4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de cursos en metodologías de aprendizaje e investigación. En caso de no disponer de cursos poner cero </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DF4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Fecha de inicio del año sabático (formato: dd/mm/yyyy). En caso que no utilizó el periodo sabático dejar en blanco
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DG4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Fecha de fin del año sabático (formato: dd/mm/yyyy). En caso que no utilizó el periodo sabático dejar en blanco
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DH4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nombre del libro publicado en el año. En caso de haber publicado más de un libro detallar en el campo observaciones. En caso de no tener poner “NO APLICA”</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DI4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Año de publicación del libro. En caso de no publicado poner cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DL4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Número de ISBN del libro publicado. En caso de no publicado poner cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DM4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Nombre de la revista donde se publicó el artículo entre el 2010 y 2012. En caso de haber publicado más de un artículo detallar en el campo observaciones. En caso de no tener artículos “NO APLICA”
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DN4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Año de publicación del artículo, si no se realizó publicaciones poner cero
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="DY4" authorId="0">
+Participación en la publicación del segundo artículo
+• AUTOR 
+• COAUTOR
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EC4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Estado de publicación del segundo artículo
+• PUBLICADO
+• ACEPTADO PARA PUBLICACIÓN
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="ED4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La revista donde publicó el segundo artículo se encuentra indexada
+• SI
+• NO
+• NO APLICA
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EE4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Base de datos en la cual esta indexada la revista de la publicación del segundo artículo
+• ISI WEB OF KONWLEDGE 
+• SCIMAGO JOURNAL RANK (SCOPUS)
+• LATIN INDEX
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EF4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El personal académico se acogió a la movilidad en instituciones de educación superior extranjeras
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EG4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El personal académico se acogió a la movilidad en instituciones de educación superior nacionales
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EH4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La institución le ofrece al personal académico un sistema informático de registro y consultas académicas
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EI4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La institución le ofrece al personal académico servicio de correo electrónico institucional
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EJ4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La institución le ofrece al personal académico el servicio de biblioteca virtual
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EK4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">La institución le ofrece al personal académico una plataforma para enseñanza virtual
+• SI
+• NO
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EL4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1428,7 +1852,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DZ4" authorId="0">
+    <comment ref="EM4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1446,7 +1870,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="144">
   <si>
     <t>CODIGO_CAMPUS</t>
   </si>
@@ -1496,9 +1920,6 @@
     <t>NUMERO_CARNET_CONADIS</t>
   </si>
   <si>
-    <t>PORCENTAJ_DISCAPACIDAD</t>
-  </si>
-  <si>
     <t>EMAIL_PERSONAL</t>
   </si>
   <si>
@@ -1763,39 +2184,6 @@
     <t>FECHA_FIN_SABATICO</t>
   </si>
   <si>
-    <t>NOMBRE_LIBRO_PUBLICADO_PERSONAL_ACADEMICO</t>
-  </si>
-  <si>
-    <t>ANIO_PUBLICACION_LIBRO</t>
-  </si>
-  <si>
-    <t>PARTICIPACION_LIBRO</t>
-  </si>
-  <si>
-    <t>REVISION_LIBRO_PARES</t>
-  </si>
-  <si>
-    <t>NUMERO_ISBN</t>
-  </si>
-  <si>
-    <t>NOMBRE_REVISTA_ARTICULO_PUBLICADO_PERSONAL_ACADEMICO</t>
-  </si>
-  <si>
-    <t>ANIO_PUBLICACION_ARTICULO</t>
-  </si>
-  <si>
-    <t>PARTICIPACION_ARTICULO</t>
-  </si>
-  <si>
-    <t>ESTADO_PUBLICACION</t>
-  </si>
-  <si>
-    <t>REVISTA_INDEXADA_PUBLICACION_ARTICULO</t>
-  </si>
-  <si>
-    <t>BASE_DATOS_REVISTA_INDEXADA</t>
-  </si>
-  <si>
     <t>MOVILIDAD_IES_EXTRANJERAS</t>
   </si>
   <si>
@@ -1835,7 +2223,82 @@
     <t>HORAS_LABORADAS_ANUALES</t>
   </si>
   <si>
-    <t>FORMULARIO PERSONAL ACADEMICO</t>
+    <t>PORCENTAJE_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>NOMBRE_LIBRO_PUBLICADO_PERSONAL_ACADEMICO_1</t>
+  </si>
+  <si>
+    <t>ANIO_PUBLICACION_LIBRO_1</t>
+  </si>
+  <si>
+    <t>PARTICIPACION_LIBRO_1</t>
+  </si>
+  <si>
+    <t>REVISION_LIBRO_PARES_1</t>
+  </si>
+  <si>
+    <t>NUMERO_ISBN_1</t>
+  </si>
+  <si>
+    <t>NOMBRE_LIBRO_PUBLICADO_PERSONAL_ACADEMICO_2</t>
+  </si>
+  <si>
+    <t>ANIO_PUBLICACION_LIBRO_2</t>
+  </si>
+  <si>
+    <t>PARTICIPACION_LIBRO_2</t>
+  </si>
+  <si>
+    <t>REVISION_LIBRO_PARES_2</t>
+  </si>
+  <si>
+    <t>NUMERO_ISBN_2</t>
+  </si>
+  <si>
+    <t>NOMBRE_REVISTA_ARTICULO_PUBLICADO_PERSONAL_ACADEMICO_1</t>
+  </si>
+  <si>
+    <t>ANIO_PUBLICACION_ARTICULO_1</t>
+  </si>
+  <si>
+    <t>PARTICIPACION_ARTICULO_1</t>
+  </si>
+  <si>
+    <t>ESTADO_PUBLICACION_1</t>
+  </si>
+  <si>
+    <t>REVISTA_INDEXADA_PUBLICACION_ARTICULO_1</t>
+  </si>
+  <si>
+    <t>BASE_DATOS_REVISTA_INDEXADA_1</t>
+  </si>
+  <si>
+    <t>NOMBRE_ARTICULO_2</t>
+  </si>
+  <si>
+    <t>NOMBRE_REVISTA_ARTICULO_PUBLICADO_PERSONAL_ACADEMICO_2</t>
+  </si>
+  <si>
+    <t>ANIO_PUBLICACION_ARTICULO_2</t>
+  </si>
+  <si>
+    <t>PARTICIPACION_ARTICULO_2</t>
+  </si>
+  <si>
+    <t>ESTADO_PUBLICACION_2</t>
+  </si>
+  <si>
+    <t>REVISTA_INDEXADA_PUBLICACION_ARTICULO_2</t>
+  </si>
+  <si>
+    <t>BASE_DATOS_REVISTA_INDEXADA_2</t>
+  </si>
+  <si>
+    <t>NOMBRE_ARTICULO_1</t>
+  </si>
+  <si>
+    <t>FORMULARIO DEL PERSONAL ACADÉMICO</t>
   </si>
   <si>
     <t>Nombre Institución:</t>
@@ -1845,7 +2308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1988,6 +2451,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2372,29 +2842,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2739,548 +3206,685 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DZ4"/>
+  <dimension ref="A1:EM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="38.140625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="46.7109375" style="3" customWidth="1"/>
-    <col min="25" max="25" width="40.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="54.28515625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="42.140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="42.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="42" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="50.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="57" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="45.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="47.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="40.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="55.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="46.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="63" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="50.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="39.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="32.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="38.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="47.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="38.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="35.85546875" style="3" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="55" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="42.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="42.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="36" style="3" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="42.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="50.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="41.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="58.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="46" style="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="47.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="48.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="47.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="55.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="46.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="63.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="39.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="36.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="24.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="25.28515625" style="3" customWidth="1"/>
-    <col min="73" max="73" width="26" style="3" customWidth="1"/>
-    <col min="74" max="74" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="34.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="31.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="43.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="35.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="21.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="32.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="28" style="3" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="20.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="37" style="3" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="22.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="33.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="51.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="22.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="64.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="30.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="25.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="22.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="44.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="33.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="30.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="29.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="45.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="38.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="35.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="28.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="41.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="38.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="32.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="45.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="37.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="52.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="42.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="43.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="37.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="50" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="42.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="57.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="47" style="7" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="35" style="7" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="36.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="41.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="34.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="44.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="49.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="42.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="37.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="40" style="7" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="45.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="44.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="37.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="52.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="42.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="43.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="45.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="51.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="58.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="47" style="7" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="19.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="22.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="34.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="22" style="7" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="23.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="24.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="23.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="38.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="30" style="7" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="30" style="7" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="30" style="7" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="35.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="39.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="17.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="30.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="34.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="23.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="36.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="34.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="20.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="30.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="25.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="50.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="31" style="7" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="26" style="7" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="28" style="7" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="50" style="7" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="23.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="23.7109375" style="7" customWidth="1"/>
+    <col min="122" max="122" width="35.7109375" style="7" customWidth="1"/>
+    <col min="123" max="123" width="61.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="35.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="25.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="42" style="7" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="39.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="39.140625" style="7" customWidth="1"/>
+    <col min="130" max="130" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="62" style="7" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="38.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="25.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="42.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="39.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="31" style="7" bestFit="1" customWidth="1"/>
+    <col min="139" max="140" width="42.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="35.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="33.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="26" style="7" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="154" max="161" width="11.42578125" style="1"/>
+    <col min="162" max="163" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="166" max="171" width="11.42578125" style="1"/>
+    <col min="172" max="172" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="173" max="175" width="11.42578125" style="1"/>
+    <col min="176" max="176" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="11.42578125" style="1"/>
+    <col min="183" max="183" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="11.42578125" style="1"/>
+    <col min="185" max="185" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="11.42578125" style="1"/>
+    <col min="188" max="190" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="192" max="195" width="11.42578125" style="1"/>
+    <col min="196" max="196" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="197" max="200" width="11.42578125" style="1"/>
+    <col min="201" max="201" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="202" max="203" width="11.42578125" style="1"/>
+    <col min="204" max="205" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="209" max="211" width="11.42578125" style="1"/>
+    <col min="212" max="212" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="213" max="214" width="11.42578125" style="1"/>
+    <col min="215" max="215" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="219" max="221" width="11.42578125" style="1"/>
+    <col min="222" max="222" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="223" max="224" width="11.42578125" style="1"/>
+    <col min="225" max="226" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="230" max="232" width="11.42578125" style="1"/>
+    <col min="233" max="233" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="234" max="236" width="11.42578125" style="1"/>
+    <col min="237" max="237" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="238" max="240" width="11.42578125" style="1"/>
+    <col min="241" max="241" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="242" max="244" width="11.42578125" style="1"/>
+    <col min="245" max="245" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="249" max="251" width="11.42578125" style="1"/>
+    <col min="252" max="252" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="253" max="255" width="11.42578125" style="1"/>
+    <col min="256" max="256" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="257" max="259" width="11.42578125" style="1"/>
+    <col min="260" max="260" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="261" max="263" width="11.42578125" style="1"/>
+    <col min="264" max="264" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="265" max="266" width="11.42578125" style="1"/>
+    <col min="267" max="267" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="268" max="269" width="11.42578125" style="1"/>
+    <col min="270" max="270" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="271" max="272" width="11.42578125" style="1"/>
+    <col min="273" max="273" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="274" max="275" width="11.42578125" style="1"/>
+    <col min="276" max="276" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="277" max="278" width="11.42578125" style="1"/>
+    <col min="279" max="279" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="280" max="281" width="11.42578125" style="1"/>
+    <col min="282" max="282" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="284" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:130" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1"/>
-      <c r="O1"/>
-      <c r="P1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
-      <c r="Z1"/>
-      <c r="AA1"/>
-      <c r="AB1"/>
-      <c r="AC1"/>
-      <c r="AD1"/>
-      <c r="AE1"/>
-      <c r="AF1"/>
-      <c r="AG1"/>
-      <c r="AH1"/>
-      <c r="AI1"/>
-      <c r="AJ1"/>
-      <c r="AK1"/>
-      <c r="AL1"/>
-      <c r="AM1"/>
-      <c r="AN1"/>
-      <c r="AO1"/>
-      <c r="AP1"/>
-      <c r="AQ1"/>
-      <c r="AR1"/>
-      <c r="AS1"/>
-      <c r="AT1"/>
-      <c r="AU1"/>
-      <c r="AV1"/>
-      <c r="AW1"/>
-      <c r="AX1"/>
-      <c r="AY1"/>
-      <c r="AZ1"/>
-      <c r="BA1"/>
-      <c r="BB1"/>
-      <c r="BC1"/>
-      <c r="BD1"/>
-      <c r="BE1"/>
-      <c r="BF1"/>
-      <c r="BG1"/>
-      <c r="BH1"/>
-      <c r="BI1"/>
-      <c r="BJ1"/>
-      <c r="BK1"/>
-      <c r="BL1"/>
-      <c r="BM1"/>
-      <c r="BN1"/>
-      <c r="BO1"/>
-      <c r="BP1"/>
-      <c r="BQ1"/>
-      <c r="BR1"/>
-      <c r="BS1"/>
-      <c r="BT1"/>
-      <c r="BU1"/>
-      <c r="BV1"/>
-      <c r="BW1"/>
-      <c r="BX1"/>
-      <c r="BY1"/>
-      <c r="BZ1"/>
-      <c r="CA1"/>
-      <c r="CB1"/>
-      <c r="CC1"/>
-      <c r="CD1"/>
-      <c r="CE1"/>
-      <c r="CF1"/>
-      <c r="CG1"/>
-      <c r="CH1"/>
-      <c r="CI1"/>
-      <c r="CJ1"/>
-      <c r="CK1"/>
-      <c r="CL1"/>
-      <c r="CM1"/>
-      <c r="CN1"/>
-      <c r="CO1"/>
-      <c r="CP1"/>
-      <c r="CQ1"/>
-      <c r="CR1"/>
-      <c r="CS1"/>
-      <c r="CT1"/>
-      <c r="CU1"/>
-      <c r="CV1"/>
-      <c r="CW1"/>
-      <c r="CX1"/>
-      <c r="CY1"/>
-      <c r="CZ1"/>
-      <c r="DA1"/>
-      <c r="DB1"/>
-      <c r="DC1"/>
-      <c r="DD1"/>
-      <c r="DE1"/>
-      <c r="DF1"/>
-      <c r="DG1"/>
-      <c r="DH1"/>
-      <c r="DI1"/>
-      <c r="DJ1"/>
-      <c r="DK1"/>
-      <c r="DL1"/>
-      <c r="DM1"/>
-      <c r="DN1"/>
-      <c r="DO1"/>
-      <c r="DP1"/>
-      <c r="DQ1"/>
-      <c r="DR1"/>
-      <c r="DS1"/>
-      <c r="DT1"/>
-      <c r="DU1"/>
-      <c r="DV1"/>
-      <c r="DW1"/>
-      <c r="DX1"/>
-      <c r="DY1"/>
-      <c r="DZ1"/>
+        <v>142</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
+      <c r="BD1" s="1"/>
+      <c r="BE1" s="1"/>
+      <c r="BF1" s="1"/>
+      <c r="BG1" s="1"/>
+      <c r="BH1" s="1"/>
+      <c r="BI1" s="1"/>
+      <c r="BJ1" s="1"/>
+      <c r="BK1" s="1"/>
+      <c r="BL1" s="1"/>
+      <c r="BM1" s="1"/>
+      <c r="BN1" s="1"/>
+      <c r="BO1" s="1"/>
+      <c r="BP1" s="1"/>
+      <c r="BQ1" s="1"/>
+      <c r="BR1" s="1"/>
+      <c r="BS1" s="1"/>
+      <c r="BT1" s="1"/>
+      <c r="BU1" s="1"/>
+      <c r="BV1" s="1"/>
+      <c r="BW1" s="1"/>
+      <c r="BX1" s="1"/>
+      <c r="BY1" s="1"/>
+      <c r="BZ1" s="1"/>
+      <c r="CA1" s="1"/>
+      <c r="CB1" s="1"/>
+      <c r="CC1" s="1"/>
+      <c r="CD1" s="1"/>
+      <c r="CE1" s="1"/>
+      <c r="CF1" s="1"/>
+      <c r="CG1" s="1"/>
+      <c r="CH1" s="1"/>
+      <c r="CI1" s="1"/>
+      <c r="CJ1" s="1"/>
+      <c r="CK1" s="1"/>
+      <c r="CL1" s="1"/>
+      <c r="CM1" s="1"/>
+      <c r="CN1" s="1"/>
+      <c r="CO1" s="1"/>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
+      <c r="CT1" s="1"/>
+      <c r="CU1" s="1"/>
+      <c r="CV1" s="1"/>
+      <c r="CW1" s="1"/>
+      <c r="CX1" s="1"/>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
+      <c r="DC1" s="1"/>
+      <c r="DD1" s="1"/>
+      <c r="DE1" s="1"/>
+      <c r="DF1" s="1"/>
+      <c r="DG1" s="1"/>
+      <c r="DH1" s="1"/>
+      <c r="DI1" s="1"/>
+      <c r="DJ1" s="1"/>
+      <c r="DK1" s="1"/>
+      <c r="DL1" s="1"/>
+      <c r="DM1" s="1"/>
+      <c r="DN1" s="1"/>
+      <c r="DO1" s="1"/>
+      <c r="DP1" s="1"/>
+      <c r="DQ1" s="1"/>
+      <c r="DR1" s="1"/>
+      <c r="DS1" s="1"/>
+      <c r="DT1" s="1"/>
+      <c r="DU1" s="1"/>
+      <c r="DV1" s="1"/>
+      <c r="DW1" s="1"/>
+      <c r="DX1" s="1"/>
+      <c r="DY1" s="1"/>
+      <c r="DZ1" s="1"/>
+      <c r="EA1" s="1"/>
+      <c r="EB1" s="1"/>
+      <c r="EC1" s="1"/>
+      <c r="ED1" s="1"/>
+      <c r="EE1" s="1"/>
+      <c r="EF1" s="1"/>
+      <c r="EG1" s="1"/>
+      <c r="EH1" s="1"/>
+      <c r="EI1" s="1"/>
+      <c r="EJ1" s="1"/>
+      <c r="EK1" s="1"/>
+      <c r="EL1" s="1"/>
+      <c r="EM1" s="1"/>
     </row>
-    <row r="2" spans="1:130" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2"/>
-      <c r="AR2"/>
-      <c r="AS2"/>
-      <c r="AT2"/>
-      <c r="AU2"/>
-      <c r="AV2"/>
-      <c r="AW2"/>
-      <c r="AX2"/>
-      <c r="AY2"/>
-      <c r="AZ2"/>
-      <c r="BA2"/>
-      <c r="BB2"/>
-      <c r="BC2"/>
-      <c r="BD2"/>
-      <c r="BE2"/>
-      <c r="BF2"/>
-      <c r="BG2"/>
-      <c r="BH2"/>
-      <c r="BI2"/>
-      <c r="BJ2"/>
-      <c r="BK2"/>
-      <c r="BL2"/>
-      <c r="BM2" s="4"/>
-      <c r="BN2" s="4"/>
-      <c r="BO2"/>
-      <c r="BP2"/>
-      <c r="BQ2"/>
-      <c r="BR2"/>
-      <c r="BS2"/>
-      <c r="BT2"/>
-      <c r="BU2"/>
-      <c r="BV2"/>
-      <c r="BW2"/>
-      <c r="BX2"/>
-      <c r="BY2"/>
-      <c r="BZ2"/>
-      <c r="CA2"/>
-      <c r="CB2"/>
-      <c r="CC2"/>
-      <c r="CD2"/>
-      <c r="CE2"/>
-      <c r="CF2"/>
-      <c r="CG2"/>
-      <c r="CH2"/>
-      <c r="CI2"/>
-      <c r="CJ2"/>
-      <c r="CK2"/>
-      <c r="CL2"/>
-      <c r="CM2"/>
-      <c r="CN2"/>
-      <c r="CO2"/>
-      <c r="CP2"/>
-      <c r="CQ2"/>
-      <c r="CR2"/>
-      <c r="CS2"/>
-      <c r="CT2"/>
-      <c r="CU2"/>
-      <c r="CV2"/>
-      <c r="CW2"/>
-      <c r="CX2"/>
-      <c r="CY2"/>
-      <c r="CZ2"/>
-      <c r="DA2"/>
-      <c r="DB2"/>
-      <c r="DC2"/>
-      <c r="DD2"/>
-      <c r="DE2"/>
-      <c r="DF2"/>
-      <c r="DG2"/>
-      <c r="DH2"/>
-      <c r="DI2"/>
-      <c r="DJ2"/>
-      <c r="DK2"/>
-      <c r="DL2"/>
-      <c r="DM2"/>
-      <c r="DN2"/>
-      <c r="DO2"/>
-      <c r="DP2"/>
-      <c r="DQ2"/>
-      <c r="DR2"/>
-      <c r="DS2"/>
-      <c r="DT2"/>
-      <c r="DU2"/>
-      <c r="DV2"/>
-      <c r="DW2"/>
-      <c r="DX2"/>
-      <c r="DY2"/>
-      <c r="DZ2"/>
+    <row r="2" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1"/>
+      <c r="BR2" s="1"/>
+      <c r="BS2" s="1"/>
+      <c r="BT2" s="1"/>
+      <c r="BU2" s="1"/>
+      <c r="BV2" s="1"/>
+      <c r="BW2" s="1"/>
+      <c r="BX2" s="1"/>
+      <c r="BY2" s="1"/>
+      <c r="BZ2" s="1"/>
+      <c r="CA2" s="1"/>
+      <c r="CB2" s="1"/>
+      <c r="CC2" s="1"/>
+      <c r="CD2" s="1"/>
+      <c r="CE2" s="1"/>
+      <c r="CF2" s="1"/>
+      <c r="CG2" s="1"/>
+      <c r="CH2" s="1"/>
+      <c r="CI2" s="1"/>
+      <c r="CJ2" s="1"/>
+      <c r="CK2" s="1"/>
+      <c r="CL2" s="1"/>
+      <c r="CM2" s="1"/>
+      <c r="CN2" s="1"/>
+      <c r="CO2" s="1"/>
+      <c r="CP2" s="1"/>
+      <c r="CQ2" s="1"/>
+      <c r="CR2" s="1"/>
+      <c r="CS2" s="1"/>
+      <c r="CT2" s="1"/>
+      <c r="CU2" s="1"/>
+      <c r="CV2" s="1"/>
+      <c r="CW2" s="1"/>
+      <c r="CX2" s="1"/>
+      <c r="CY2" s="1"/>
+      <c r="CZ2" s="1"/>
+      <c r="DA2" s="1"/>
+      <c r="DB2" s="1"/>
+      <c r="DC2" s="1"/>
+      <c r="DD2" s="1"/>
+      <c r="DE2" s="1"/>
+      <c r="DF2" s="1"/>
+      <c r="DG2" s="1"/>
+      <c r="DH2" s="1"/>
+      <c r="DI2" s="1"/>
+      <c r="DJ2" s="1"/>
+      <c r="DK2" s="1"/>
+      <c r="DL2" s="1"/>
+      <c r="DM2" s="1"/>
+      <c r="DN2" s="1"/>
+      <c r="DO2" s="1"/>
+      <c r="DP2" s="1"/>
+      <c r="DQ2" s="1"/>
+      <c r="DR2" s="1"/>
+      <c r="DS2" s="1"/>
+      <c r="DT2" s="1"/>
+      <c r="DU2" s="1"/>
+      <c r="DV2" s="1"/>
+      <c r="DW2" s="1"/>
+      <c r="DX2" s="1"/>
+      <c r="DY2" s="1"/>
+      <c r="DZ2" s="1"/>
+      <c r="EA2" s="1"/>
+      <c r="EB2" s="1"/>
+      <c r="EC2" s="1"/>
+      <c r="ED2" s="1"/>
+      <c r="EE2" s="1"/>
+      <c r="EF2" s="1"/>
+      <c r="EG2" s="1"/>
+      <c r="EH2" s="1"/>
+      <c r="EI2" s="1"/>
+      <c r="EJ2" s="1"/>
+      <c r="EK2" s="1"/>
+      <c r="EL2" s="1"/>
+      <c r="EM2" s="1"/>
     </row>
-    <row r="3" spans="1:130" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
-      <c r="U3"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3"/>
-      <c r="AF3"/>
-      <c r="AG3"/>
-      <c r="AH3"/>
-      <c r="AI3"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
-      <c r="AL3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
-      <c r="AS3"/>
-      <c r="AT3"/>
-      <c r="AU3"/>
-      <c r="AV3"/>
-      <c r="AW3"/>
-      <c r="AX3"/>
-      <c r="AY3"/>
-      <c r="AZ3"/>
-      <c r="BA3"/>
-      <c r="BB3"/>
-      <c r="BC3"/>
-      <c r="BD3"/>
-      <c r="BE3"/>
-      <c r="BF3"/>
-      <c r="BG3"/>
-      <c r="BH3"/>
-      <c r="BI3"/>
-      <c r="BJ3"/>
-      <c r="BK3"/>
-      <c r="BL3"/>
-      <c r="BM3"/>
-      <c r="BN3"/>
-      <c r="BO3"/>
-      <c r="BP3"/>
-      <c r="BQ3"/>
-      <c r="BR3"/>
-      <c r="BS3"/>
-      <c r="BT3"/>
-      <c r="BU3"/>
-      <c r="BV3"/>
-      <c r="BW3"/>
-      <c r="BX3"/>
-      <c r="BY3"/>
-      <c r="BZ3"/>
-      <c r="CA3"/>
-      <c r="CB3"/>
-      <c r="CC3"/>
-      <c r="CD3"/>
-      <c r="CE3"/>
-      <c r="CF3"/>
-      <c r="CG3"/>
-      <c r="CH3"/>
-      <c r="CI3"/>
-      <c r="CJ3"/>
-      <c r="CK3"/>
-      <c r="CL3"/>
-      <c r="CM3"/>
-      <c r="CN3"/>
-      <c r="CO3"/>
-      <c r="CP3"/>
-      <c r="CQ3"/>
-      <c r="CR3"/>
-      <c r="CS3"/>
-      <c r="CT3"/>
-      <c r="CU3"/>
-      <c r="CV3"/>
-      <c r="CW3"/>
-      <c r="CX3"/>
-      <c r="CY3"/>
-      <c r="CZ3"/>
-      <c r="DA3"/>
-      <c r="DB3"/>
-      <c r="DC3"/>
-      <c r="DD3"/>
-      <c r="DE3"/>
-      <c r="DF3"/>
-      <c r="DG3"/>
-      <c r="DH3"/>
-      <c r="DI3"/>
-      <c r="DJ3"/>
-      <c r="DK3"/>
-      <c r="DL3"/>
-      <c r="DM3"/>
-      <c r="DN3"/>
-      <c r="DO3"/>
-      <c r="DP3"/>
-      <c r="DQ3"/>
-      <c r="DR3"/>
-      <c r="DS3"/>
-      <c r="DT3"/>
-      <c r="DU3"/>
-      <c r="DV3"/>
-      <c r="DW3"/>
-      <c r="DX3"/>
-      <c r="DY3"/>
-      <c r="DZ3"/>
+    <row r="3" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="1"/>
+      <c r="BC3" s="1"/>
+      <c r="BD3" s="1"/>
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1"/>
+      <c r="BJ3" s="1"/>
+      <c r="BK3" s="1"/>
+      <c r="BL3" s="1"/>
+      <c r="BM3" s="1"/>
+      <c r="BN3" s="1"/>
+      <c r="BO3" s="1"/>
+      <c r="BP3" s="1"/>
+      <c r="BQ3" s="1"/>
+      <c r="BR3" s="1"/>
+      <c r="BS3" s="1"/>
+      <c r="BT3" s="1"/>
+      <c r="BU3" s="1"/>
+      <c r="BV3" s="1"/>
+      <c r="BW3" s="1"/>
+      <c r="BX3" s="1"/>
+      <c r="BY3" s="1"/>
+      <c r="BZ3" s="1"/>
+      <c r="CA3" s="1"/>
+      <c r="CB3" s="1"/>
+      <c r="CC3" s="1"/>
+      <c r="CD3" s="1"/>
+      <c r="CE3" s="1"/>
+      <c r="CF3" s="1"/>
+      <c r="CG3" s="1"/>
+      <c r="CH3" s="1"/>
+      <c r="CI3" s="1"/>
+      <c r="CJ3" s="1"/>
+      <c r="CK3" s="1"/>
+      <c r="CL3" s="1"/>
+      <c r="CM3" s="1"/>
+      <c r="CN3" s="1"/>
+      <c r="CO3" s="1"/>
+      <c r="CP3" s="1"/>
+      <c r="CQ3" s="1"/>
+      <c r="CR3" s="1"/>
+      <c r="CS3" s="1"/>
+      <c r="CT3" s="1"/>
+      <c r="CU3" s="1"/>
+      <c r="CV3" s="1"/>
+      <c r="CW3" s="1"/>
+      <c r="CX3" s="1"/>
+      <c r="CY3" s="1"/>
+      <c r="CZ3" s="1"/>
+      <c r="DA3" s="1"/>
+      <c r="DB3" s="1"/>
+      <c r="DC3" s="1"/>
+      <c r="DD3" s="1"/>
+      <c r="DE3" s="1"/>
+      <c r="DF3" s="1"/>
+      <c r="DG3" s="1"/>
+      <c r="DH3" s="1"/>
+      <c r="DI3" s="1"/>
+      <c r="DJ3" s="1"/>
+      <c r="DK3" s="1"/>
+      <c r="DL3" s="1"/>
+      <c r="DM3" s="1"/>
+      <c r="DN3" s="1"/>
+      <c r="DO3" s="1"/>
+      <c r="DP3" s="1"/>
+      <c r="DQ3" s="1"/>
+      <c r="DR3" s="1"/>
+      <c r="DS3" s="1"/>
+      <c r="DT3" s="1"/>
+      <c r="DU3" s="1"/>
+      <c r="DV3" s="1"/>
+      <c r="DW3" s="1"/>
+      <c r="DX3" s="1"/>
+      <c r="DY3" s="1"/>
+      <c r="DZ3" s="1"/>
+      <c r="EA3" s="1"/>
+      <c r="EB3" s="1"/>
+      <c r="EC3" s="1"/>
+      <c r="ED3" s="1"/>
+      <c r="EE3" s="1"/>
+      <c r="EF3" s="1"/>
+      <c r="EG3" s="1"/>
+      <c r="EH3" s="1"/>
+      <c r="EI3" s="1"/>
+      <c r="EJ3" s="1"/>
+      <c r="EK3" s="1"/>
+      <c r="EL3" s="1"/>
+      <c r="EM3" s="1"/>
     </row>
-    <row r="4" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3309,10 +3913,10 @@
         <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>9</v>
@@ -3336,90 +3940,92 @@
         <v>15</v>
       </c>
       <c r="S4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AI4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AK4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP4" s="1" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="AU4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU4" s="1"/>
       <c r="AV4" s="1" t="s">
         <v>44</v>
       </c>
@@ -3481,22 +4087,22 @@
         <v>63</v>
       </c>
       <c r="BP4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="BQ4" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="BQ4" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="BR4" s="1" t="s">
         <v>65</v>
       </c>
       <c r="BS4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BT4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU4" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="BT4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BU4" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="BV4" s="1" t="s">
         <v>67</v>
@@ -3610,70 +4216,108 @@
         <v>103</v>
       </c>
       <c r="DG4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DH4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DI4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DJ4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DK4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DL4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DM4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DN4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DO4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DP4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DQ4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DR4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DS4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DT4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DU4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DV4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DW4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DX4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DY4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DZ4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EA4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EB4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EC4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="ED4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EE4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EF4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DH4" s="1" t="s">
+      <c r="EG4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DI4" s="1" t="s">
+      <c r="EH4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DJ4" s="1" t="s">
+      <c r="EI4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DK4" s="1" t="s">
+      <c r="EJ4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DL4" s="1" t="s">
+      <c r="EK4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DM4" s="1" t="s">
+      <c r="EL4" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DN4" s="1" t="s">
+      <c r="EM4" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="DO4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DP4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DQ4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="DR4" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="DS4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="DT4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="DU4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="DV4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="DW4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="DX4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="DY4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="DZ4" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection password="E801" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="3">
-    <mergeCell ref="BM2:BN2"/>
+  <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:E2"/>
   </mergeCells>

</xml_diff>

<commit_message>
actualizacion manual y PAC 2011 y 2012
</commit_message>
<xml_diff>
--- a/public_html/archivos/2011_PAC.xlsx
+++ b/public_html/archivos/2011_PAC.xlsx
@@ -850,7 +850,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Número total de horas laboradas al año.</t>
+          <t>Número total de horas clases laboradas al año del nombramiento o contrato que se encuentra registrando.</t>
         </r>
       </text>
     </comment>
@@ -1133,6 +1133,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="CJ4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">El personal académico ocupa uno de los siguientes cargos de autoridad:
+• RECTOR(A)
+• VICERRECTOR(A)
+• DECANO(A)
+• SUBDECANO(A)
+• COORDINADOR(A)
+• DIRECTOR(A)
+• JEFE(A) DEPARTAMENTAL
+• NINGUNO
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="CK4" authorId="0">
       <text>
         <r>
@@ -1142,7 +1164,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Fecha inicio del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 dejar en blanco
+          <t xml:space="preserve">Fecha inicio del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta anterior dejar en blanco
 </t>
         </r>
       </text>
@@ -1156,7 +1178,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Fecha de finalización del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta 17 dejar en blanco
+          <t xml:space="preserve">Fecha de finalización del cargo de autoridad, en caso de haber seleccionado “ninguno” en la pregunta anterior  dejar en blanco
 </t>
         </r>
       </text>
@@ -1198,8 +1220,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal a la docencia. 
-</t>
+          <t>Horas de dedicación por semana según Contrato o Nombramiento, no registrar las horas adicionales a las firmadas en el contrato o nombramiento</t>
         </r>
       </text>
     </comment>
@@ -1212,7 +1233,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal a la docencia. 
+          <t xml:space="preserve">Número de horas de investigación en el periodo del contrato. Cuando la contratación es durante todo el año se debe especificar el número de horas totales en el año.
+Si durante el periodo de análisis (2011 o 2012) el docente tuvo varios contratos debe especificarse por cada contrato las horas de dedicación. En caso que no se disponga de horas de investigación poner 0
 </t>
         </r>
       </text>
@@ -1226,8 +1248,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dirección o gestión administrativa
-</t>
+          <t>Número de horas en gestión  administrativa en el periodo del contrato. Cuando la contratación es durante todo el año se debe especificar el número de horas totales en el año.
+Si durante el periodo de análisis  (2011 o 2012) el docente tuvo varios contratos debe especificarse por cada contrato las horas de dedicación. En caso que no se disponga de horas administrativas poner 0</t>
         </r>
       </text>
     </comment>
@@ -1240,12 +1262,39 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Número de horas de dedicación semanal a vinculación con la sociedad. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="CU4" authorId="0">
+          <t xml:space="preserve">Número de horas dedicadas a la  vinculación con la sociedad en el periodo del contrato. Cuando la contratación es durante todo el año se debe especificar el Número de horas totales en el año.
+Si durante el periodo de análisis  (2011 o 2012) el docente tuvo varios contratos debe especificarse por cada contrato las horas de dedicación En caso que no se disponga de horas de vinculación con la sociedad poner 0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CU4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Número de horas dedicadas a otras actividades. Si no realiza otras actividades poner 0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CV4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Especificar todas las otras actividades que realiza el docente. Si no realiza otras actividades poner NO APLICA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CW4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1259,7 +1308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CV4" authorId="0">
+    <comment ref="CX4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1273,7 +1322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CW4" authorId="0">
+    <comment ref="CY4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1287,7 +1336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CX4" authorId="0">
+    <comment ref="CZ4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1301,7 +1350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CY4" authorId="0">
+    <comment ref="DA4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1315,7 +1364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CZ4" authorId="0">
+    <comment ref="DB4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1329,7 +1378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DA4" authorId="0">
+    <comment ref="DC4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1342,7 +1391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DE4" authorId="0">
+    <comment ref="DG4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DF4" authorId="0">
+    <comment ref="DH4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1370,7 +1419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DG4" authorId="0">
+    <comment ref="DI4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1383,7 +1432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DH4" authorId="0">
+    <comment ref="DJ4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1396,7 +1445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DI4" authorId="1">
+    <comment ref="DK4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1413,7 +1462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DJ4" authorId="1">
+    <comment ref="DL4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1429,7 +1478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DK4" authorId="0">
+    <comment ref="DM4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1442,7 +1491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DL4" authorId="0">
+    <comment ref="DN4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1455,7 +1504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DM4" authorId="0">
+    <comment ref="DO4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1468,7 +1517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DN4" authorId="1">
+    <comment ref="DP4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1485,7 +1534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DO4" authorId="1">
+    <comment ref="DQ4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1501,7 +1550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DP4" authorId="0">
+    <comment ref="DR4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1514,7 +1563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DQ4" authorId="1">
+    <comment ref="DS4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1527,7 +1576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DR4" authorId="0">
+    <comment ref="DT4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1540,7 +1589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DS4" authorId="0">
+    <comment ref="DU4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1553,7 +1602,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DT4" authorId="1">
+    <comment ref="DV4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1570,7 +1619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DU4" authorId="1">
+    <comment ref="DW4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1587,7 +1636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DV4" authorId="1">
+    <comment ref="DX4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1604,7 +1653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DW4" authorId="1">
+    <comment ref="DY4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1621,7 +1670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DX4" authorId="1">
+    <comment ref="DZ4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1634,7 +1683,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DY4" authorId="1">
+    <comment ref="EA4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1647,7 +1696,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DZ4" authorId="1">
+    <comment ref="EB4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1660,7 +1709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EA4" authorId="1">
+    <comment ref="EC4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1673,7 +1722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EB4" authorId="1">
+    <comment ref="ED4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1691,7 +1740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EC4" authorId="1">
+    <comment ref="EE4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1708,7 +1757,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="ED4" authorId="1">
+    <comment ref="EF4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1725,7 +1774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EE4" authorId="1">
+    <comment ref="EG4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1742,7 +1791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EF4" authorId="1">
+    <comment ref="EH4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1758,7 +1807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EG4" authorId="1">
+    <comment ref="EI4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1774,7 +1823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EH4" authorId="1">
+    <comment ref="EJ4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1790,7 +1839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI4" authorId="1">
+    <comment ref="EK4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1806,7 +1855,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EJ4" authorId="1">
+    <comment ref="EL4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1822,7 +1871,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EK4" authorId="1">
+    <comment ref="EM4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1838,7 +1887,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EL4" authorId="0">
+    <comment ref="EN4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1852,7 +1901,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EM4" authorId="0">
+    <comment ref="EO4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1870,7 +1919,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="146">
   <si>
     <t>CODIGO_CAMPUS</t>
   </si>
@@ -2136,9 +2185,6 @@
     <t>UNIDAD_ACADEMICA</t>
   </si>
   <si>
-    <t>HORAS_DOCENCIA</t>
-  </si>
-  <si>
     <t>HORAS_INVESTIGACION</t>
   </si>
   <si>
@@ -2296,6 +2342,15 @@
   </si>
   <si>
     <t>NOMBRE_ARTICULO_1</t>
+  </si>
+  <si>
+    <t>HORAS_DEDICACION</t>
+  </si>
+  <si>
+    <t>HORAS_OTRAS_ACTIVIDADES</t>
+  </si>
+  <si>
+    <t>OTRAS_ACTIVIDADES</t>
   </si>
   <si>
     <t>FORMULARIO DEL PERSONAL ACADÉMICO</t>
@@ -2645,7 +2700,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2761,6 +2816,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -2842,22 +2906,25 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -3206,7 +3273,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EM4"/>
+  <dimension ref="A1:EO4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3215,239 +3282,242 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="36" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="41.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="49.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="38.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="32.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="45.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="37.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="52.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="42.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="43.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="37.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="50" style="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="42.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="57.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="47" style="7" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="35" style="7" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="36.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="41.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="34.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="44.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="49.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="42.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="37.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="40" style="7" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="45.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="44.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="37.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="52.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="42.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="43.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="44.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="45.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="51.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="58.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="28.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="47" style="7" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="19.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="22.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="34.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="22" style="7" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="23.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="24.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="23.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="38.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="30" style="7" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="30" style="7" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="35.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="30" style="7" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="35.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="39.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="17.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="30.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="34.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="23.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="36.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="34.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="30.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="20.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="30.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="25.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="50.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="31" style="7" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="26" style="7" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="50" style="7" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="23.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="23.7109375" style="7" customWidth="1"/>
-    <col min="122" max="122" width="35.7109375" style="7" customWidth="1"/>
-    <col min="123" max="123" width="61.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="35.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="28.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="25.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="42" style="7" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="39.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="39.140625" style="7" customWidth="1"/>
-    <col min="130" max="130" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="62" style="7" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="38.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="28.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="25.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="42.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="39.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="31" style="7" bestFit="1" customWidth="1"/>
-    <col min="139" max="140" width="42.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="35.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="33.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="26" style="7" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="154" max="161" width="11.42578125" style="1"/>
-    <col min="162" max="163" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="171" width="11.42578125" style="1"/>
-    <col min="172" max="172" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="173" max="175" width="11.42578125" style="1"/>
-    <col min="176" max="176" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="11.42578125" style="1"/>
-    <col min="183" max="183" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" style="8" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21" style="8" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="25" style="8" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="14" style="8" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27" style="8" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" style="8" customWidth="1"/>
+    <col min="21" max="21" width="36.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29" style="8" customWidth="1"/>
+    <col min="23" max="23" width="35.85546875" style="8" customWidth="1"/>
+    <col min="24" max="24" width="43.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="50.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="39.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.5703125" style="8" customWidth="1"/>
+    <col min="31" max="31" width="47.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="53.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="43" style="8" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="44.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="38" style="8" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="44.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="51.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="43.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="59" style="8" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="47.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="30.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="44.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="35.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="40.140625" style="8" customWidth="1"/>
+    <col min="49" max="49" width="40.28515625" style="8" customWidth="1"/>
+    <col min="50" max="50" width="34" style="8" customWidth="1"/>
+    <col min="51" max="51" width="40.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="47.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="39.140625" style="8" customWidth="1"/>
+    <col min="54" max="54" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="43.42578125" style="8" customWidth="1"/>
+    <col min="56" max="56" width="45.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="46.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="45.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="52.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="44" style="8" customWidth="1"/>
+    <col min="61" max="61" width="59.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.28515625" style="8" customWidth="1"/>
+    <col min="63" max="63" width="37.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="19.28515625" style="8" customWidth="1"/>
+    <col min="65" max="65" width="22.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20" style="8" customWidth="1"/>
+    <col min="67" max="67" width="35" style="8" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="28.42578125" style="8" customWidth="1"/>
+    <col min="69" max="69" width="23" style="8" customWidth="1"/>
+    <col min="70" max="70" width="17.7109375" style="8" customWidth="1"/>
+    <col min="71" max="71" width="24.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="25" style="8" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="29.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="21" style="8" customWidth="1"/>
+    <col min="75" max="75" width="31.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="29.42578125" style="8" customWidth="1"/>
+    <col min="77" max="77" width="21" style="8" customWidth="1"/>
+    <col min="78" max="78" width="31.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="29.42578125" style="8" customWidth="1"/>
+    <col min="80" max="80" width="21" style="8" customWidth="1"/>
+    <col min="81" max="81" width="31.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.42578125" style="8" customWidth="1"/>
+    <col min="83" max="83" width="21" style="8" customWidth="1"/>
+    <col min="84" max="84" width="31.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="29.42578125" style="8" customWidth="1"/>
+    <col min="86" max="86" width="21" style="8" customWidth="1"/>
+    <col min="87" max="87" width="31.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="19" style="8" customWidth="1"/>
+    <col min="89" max="89" width="32.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="30" style="8" customWidth="1"/>
+    <col min="91" max="91" width="41.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="33.85546875" style="8" customWidth="1"/>
+    <col min="93" max="93" width="20.140625" style="8" customWidth="1"/>
+    <col min="94" max="94" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="31" style="8" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="27.140625" style="8" customWidth="1"/>
+    <col min="100" max="100" width="19.7109375" style="8" customWidth="1"/>
+    <col min="101" max="101" width="17.7109375" style="8" customWidth="1"/>
+    <col min="102" max="102" width="22" style="8" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="27" style="8" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="19.5703125" style="8" customWidth="1"/>
+    <col min="105" max="105" width="29.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="35.140625" style="8" customWidth="1"/>
+    <col min="107" max="107" width="31.85546875" style="8" customWidth="1"/>
+    <col min="108" max="108" width="20.7109375" style="8" customWidth="1"/>
+    <col min="109" max="109" width="31.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="19" style="8" customWidth="1"/>
+    <col min="111" max="111" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="20.7109375" style="8" customWidth="1"/>
+    <col min="113" max="113" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="27.28515625" style="8" customWidth="1"/>
+    <col min="115" max="115" width="23.28515625" style="8" customWidth="1"/>
+    <col min="116" max="116" width="24.42578125" style="8" customWidth="1"/>
+    <col min="117" max="117" width="16.28515625" style="8" customWidth="1"/>
+    <col min="118" max="118" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="27.28515625" style="8" customWidth="1"/>
+    <col min="120" max="120" width="23.28515625" style="8" customWidth="1"/>
+    <col min="121" max="121" width="24.42578125" style="8" customWidth="1"/>
+    <col min="122" max="122" width="16.28515625" style="8" customWidth="1"/>
+    <col min="123" max="123" width="20.7109375" style="8" customWidth="1"/>
+    <col min="124" max="124" width="63.5703125" style="8" customWidth="1"/>
+    <col min="125" max="125" width="30.85546875" style="8" customWidth="1"/>
+    <col min="126" max="126" width="27" style="8" customWidth="1"/>
+    <col min="127" max="127" width="23.28515625" style="8" customWidth="1"/>
+    <col min="128" max="128" width="44.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="33.5703125" style="8" customWidth="1"/>
+    <col min="130" max="131" width="20.7109375" style="8" customWidth="1"/>
+    <col min="132" max="132" width="63.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="30.85546875" style="8" customWidth="1"/>
+    <col min="134" max="134" width="27" style="8" customWidth="1"/>
+    <col min="135" max="135" width="23.28515625" style="8" customWidth="1"/>
+    <col min="136" max="136" width="44.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="33.5703125" style="8" customWidth="1"/>
+    <col min="138" max="138" width="28.42578125" style="8" customWidth="1"/>
+    <col min="139" max="139" width="27.7109375" style="8" customWidth="1"/>
+    <col min="140" max="140" width="43.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="36.7109375" style="8" customWidth="1"/>
+    <col min="142" max="142" width="29.140625" style="8" customWidth="1"/>
+    <col min="143" max="143" width="34" style="8" customWidth="1"/>
+    <col min="144" max="144" width="28.5703125" style="8" customWidth="1"/>
+    <col min="145" max="145" width="36.5703125" style="8" customWidth="1"/>
+    <col min="146" max="146" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="156" max="163" width="11.42578125" style="1"/>
+    <col min="164" max="165" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="168" max="173" width="11.42578125" style="1"/>
+    <col min="174" max="174" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="175" max="177" width="11.42578125" style="1"/>
+    <col min="178" max="178" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="184" max="184" width="11.42578125" style="1"/>
-    <col min="185" max="185" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="11.42578125" style="1"/>
-    <col min="188" max="190" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="192" max="195" width="11.42578125" style="1"/>
-    <col min="196" max="196" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="197" max="200" width="11.42578125" style="1"/>
-    <col min="201" max="201" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="202" max="203" width="11.42578125" style="1"/>
-    <col min="204" max="205" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="209" max="211" width="11.42578125" style="1"/>
-    <col min="212" max="212" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="213" max="214" width="11.42578125" style="1"/>
-    <col min="215" max="215" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="219" max="221" width="11.42578125" style="1"/>
-    <col min="222" max="222" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="223" max="224" width="11.42578125" style="1"/>
-    <col min="225" max="226" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="230" max="232" width="11.42578125" style="1"/>
-    <col min="233" max="233" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="234" max="236" width="11.42578125" style="1"/>
-    <col min="237" max="237" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="238" max="240" width="11.42578125" style="1"/>
-    <col min="241" max="241" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="242" max="244" width="11.42578125" style="1"/>
-    <col min="245" max="245" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="249" max="251" width="11.42578125" style="1"/>
-    <col min="252" max="252" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="253" max="255" width="11.42578125" style="1"/>
-    <col min="256" max="256" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="257" max="259" width="11.42578125" style="1"/>
-    <col min="260" max="260" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="261" max="263" width="11.42578125" style="1"/>
-    <col min="264" max="264" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="265" max="266" width="11.42578125" style="1"/>
-    <col min="267" max="267" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="268" max="269" width="11.42578125" style="1"/>
-    <col min="270" max="270" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="271" max="272" width="11.42578125" style="1"/>
-    <col min="273" max="273" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="274" max="275" width="11.42578125" style="1"/>
-    <col min="276" max="276" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="277" max="278" width="11.42578125" style="1"/>
-    <col min="279" max="279" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="280" max="281" width="11.42578125" style="1"/>
-    <col min="282" max="282" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="284" max="16384" width="11.42578125" style="1"/>
+    <col min="185" max="185" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="11.42578125" style="1"/>
+    <col min="187" max="187" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="11.42578125" style="1"/>
+    <col min="190" max="192" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="194" max="197" width="11.42578125" style="1"/>
+    <col min="198" max="198" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="199" max="202" width="11.42578125" style="1"/>
+    <col min="203" max="203" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="204" max="205" width="11.42578125" style="1"/>
+    <col min="206" max="207" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="211" max="213" width="11.42578125" style="1"/>
+    <col min="214" max="214" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="215" max="216" width="11.42578125" style="1"/>
+    <col min="217" max="217" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="221" max="223" width="11.42578125" style="1"/>
+    <col min="224" max="224" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="225" max="226" width="11.42578125" style="1"/>
+    <col min="227" max="228" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="232" max="234" width="11.42578125" style="1"/>
+    <col min="235" max="235" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="236" max="238" width="11.42578125" style="1"/>
+    <col min="239" max="239" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="240" max="242" width="11.42578125" style="1"/>
+    <col min="243" max="243" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="244" max="246" width="11.42578125" style="1"/>
+    <col min="247" max="247" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="251" max="253" width="11.42578125" style="1"/>
+    <col min="254" max="254" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="255" max="257" width="11.42578125" style="1"/>
+    <col min="258" max="258" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="259" max="261" width="11.42578125" style="1"/>
+    <col min="262" max="262" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="263" max="265" width="11.42578125" style="1"/>
+    <col min="266" max="266" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="267" max="268" width="11.42578125" style="1"/>
+    <col min="269" max="269" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="270" max="271" width="11.42578125" style="1"/>
+    <col min="272" max="272" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="273" max="274" width="11.42578125" style="1"/>
+    <col min="275" max="275" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="276" max="277" width="11.42578125" style="1"/>
+    <col min="278" max="278" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="279" max="280" width="11.42578125" style="1"/>
+    <col min="281" max="281" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="282" max="283" width="11.42578125" style="1"/>
+    <col min="284" max="284" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="286" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:145" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3591,15 +3661,17 @@
       <c r="EK1" s="1"/>
       <c r="EL1" s="1"/>
       <c r="EM1" s="1"/>
+      <c r="EN1" s="1"/>
+      <c r="EO1" s="1"/>
     </row>
-    <row r="2" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:145" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+        <v>145</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3738,8 +3810,10 @@
       <c r="EK2" s="1"/>
       <c r="EL2" s="1"/>
       <c r="EM2" s="1"/>
+      <c r="EN2" s="1"/>
+      <c r="EO2" s="1"/>
     </row>
-    <row r="3" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3883,8 +3957,10 @@
       <c r="EK3" s="1"/>
       <c r="EL3" s="1"/>
       <c r="EM3" s="1"/>
+      <c r="EN3" s="1"/>
+      <c r="EO3" s="1"/>
     </row>
-    <row r="4" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3913,10 +3989,10 @@
         <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>9</v>
@@ -3940,7 +4016,7 @@
         <v>15</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>16</v>
@@ -4087,7 +4163,7 @@
         <v>63</v>
       </c>
       <c r="BP4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BQ4" s="1" t="s">
         <v>64</v>
@@ -4096,10 +4172,10 @@
         <v>65</v>
       </c>
       <c r="BS4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BT4" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="BT4" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="BU4" s="1" t="s">
         <v>66</v>
@@ -4168,151 +4244,157 @@
         <v>87</v>
       </c>
       <c r="CQ4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="CR4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CR4" s="1" t="s">
+      <c r="CS4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CS4" s="1" t="s">
+      <c r="CT4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CT4" s="1" t="s">
+      <c r="CU4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="CV4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="CW4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CU4" s="1" t="s">
+      <c r="CX4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CV4" s="1" t="s">
+      <c r="CY4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CW4" s="1" t="s">
+      <c r="CZ4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CX4" s="1" t="s">
+      <c r="DA4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CY4" s="1" t="s">
+      <c r="DB4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CZ4" s="1" t="s">
+      <c r="DC4" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DA4" s="1" t="s">
+      <c r="DD4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DB4" s="1" t="s">
+      <c r="DE4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="DC4" s="1" t="s">
+      <c r="DF4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="DD4" s="1" t="s">
+      <c r="DG4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="DE4" s="1" t="s">
+      <c r="DH4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DF4" s="1" t="s">
+      <c r="DI4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DJ4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DK4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DL4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DM4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DN4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DO4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DQ4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DR4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DS4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DT4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DU4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DV4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DW4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DX4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DY4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DZ4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EA4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="EB4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EC4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="ED4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EE4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="EF4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EG4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EH4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DG4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="DH4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="DI4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="DJ4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="DK4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="DL4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="DM4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="DN4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="DO4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="DP4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="DQ4" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="DR4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="DS4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="DT4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DU4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="DV4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="DW4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="DX4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="DY4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="DZ4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="EA4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="EB4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="EC4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="ED4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="EE4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="EF4" s="1" t="s">
+      <c r="EI4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="EG4" s="1" t="s">
+      <c r="EJ4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="EH4" s="1" t="s">
+      <c r="EK4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="EI4" s="1" t="s">
+      <c r="EL4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="EJ4" s="1" t="s">
+      <c r="EM4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="EK4" s="1" t="s">
+      <c r="EN4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="EL4" s="1" t="s">
+      <c r="EO4" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="EM4" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quitado campo repetido NOMBRE_ARTICULO_2 en PAC 2011 y 2012
</commit_message>
<xml_diff>
--- a/public_html/archivos/2011_PAC.xlsx
+++ b/public_html/archivos/2011_PAC.xlsx
@@ -1692,7 +1692,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Nombre del segundo artículo publicado o aceptado para la publicación, en caso de no haber publicado poner NO APLICA</t>
+          <t>Nombre de la revista donde se publicó el segundo artículo. En caso de no haber publicado el artículo poner NO APLICA</t>
         </r>
       </text>
     </comment>
@@ -1705,24 +1705,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Nombre de la revista donde se publicó el segundo artículo. En caso de no haber publicado el artículo poner NO APLICA</t>
+          <t>Año de publicación del segundo artículo. En caso de no tener publicación poner el número cero</t>
         </r>
       </text>
     </comment>
     <comment ref="EC4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Año de publicación del segundo artículo. En caso de no tener publicación poner el número cero</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="ED4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1740,7 +1727,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EE4" authorId="1">
+    <comment ref="ED4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1757,7 +1744,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EF4" authorId="1">
+    <comment ref="EE4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1774,7 +1761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EG4" authorId="1">
+    <comment ref="EF4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1791,7 +1778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EH4" authorId="1">
+    <comment ref="EG4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1807,7 +1794,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EI4" authorId="1">
+    <comment ref="EH4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1823,7 +1810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EJ4" authorId="1">
+    <comment ref="EI4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1839,7 +1826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EK4" authorId="1">
+    <comment ref="EJ4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1855,7 +1842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EL4" authorId="1">
+    <comment ref="EK4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1871,7 +1858,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="EM4" authorId="1">
+    <comment ref="EL4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1887,21 +1874,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="EM4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Correo electrónico institucional del personal académico
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="EN4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Correo electrónico institucional del personal académico
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="EO4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1919,7 +1906,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
   <si>
     <t>CODIGO_CAMPUS</t>
   </si>
@@ -2910,6 +2897,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2926,9 +2916,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3273,7 +3260,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EO4"/>
+  <dimension ref="A1:EN4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -3282,240 +3269,240 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="8" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21" style="8" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="25" style="8" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="25.7109375" style="8" customWidth="1"/>
-    <col min="13" max="13" width="14" style="8" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27" style="8" customWidth="1"/>
-    <col min="20" max="20" width="23.140625" style="8" customWidth="1"/>
-    <col min="21" max="21" width="36.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29" style="8" customWidth="1"/>
-    <col min="23" max="23" width="35.85546875" style="8" customWidth="1"/>
-    <col min="24" max="24" width="43.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="37.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="50.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="39.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="39.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="33.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="39.5703125" style="8" customWidth="1"/>
-    <col min="31" max="31" width="47.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="38.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="53.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="43" style="8" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="44.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="38" style="8" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="44.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="51.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="43.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="59" style="8" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="47.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="37.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="30.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="36.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="44.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="35.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="40.140625" style="8" customWidth="1"/>
-    <col min="49" max="49" width="40.28515625" style="8" customWidth="1"/>
-    <col min="50" max="50" width="34" style="8" customWidth="1"/>
-    <col min="51" max="51" width="40.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="47.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="39.140625" style="8" customWidth="1"/>
-    <col min="54" max="54" width="54.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="43.42578125" style="8" customWidth="1"/>
-    <col min="56" max="56" width="45.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="46.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="45.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="52.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="44" style="8" customWidth="1"/>
-    <col min="61" max="61" width="59.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="25.28515625" style="8" customWidth="1"/>
-    <col min="63" max="63" width="37.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="19.28515625" style="8" customWidth="1"/>
-    <col min="65" max="65" width="22.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="20" style="8" customWidth="1"/>
-    <col min="67" max="67" width="35" style="8" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="28.42578125" style="8" customWidth="1"/>
-    <col min="69" max="69" width="23" style="8" customWidth="1"/>
-    <col min="70" max="70" width="17.7109375" style="8" customWidth="1"/>
-    <col min="71" max="71" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="25" style="8" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="29.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="21" style="8" customWidth="1"/>
-    <col min="75" max="75" width="31.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="29.42578125" style="8" customWidth="1"/>
-    <col min="77" max="77" width="21" style="8" customWidth="1"/>
-    <col min="78" max="78" width="31.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="29.42578125" style="8" customWidth="1"/>
-    <col min="80" max="80" width="21" style="8" customWidth="1"/>
-    <col min="81" max="81" width="31.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="29.42578125" style="8" customWidth="1"/>
-    <col min="83" max="83" width="21" style="8" customWidth="1"/>
-    <col min="84" max="84" width="31.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="29.42578125" style="8" customWidth="1"/>
-    <col min="86" max="86" width="21" style="8" customWidth="1"/>
-    <col min="87" max="87" width="31.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="19" style="8" customWidth="1"/>
-    <col min="89" max="89" width="32.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="30" style="8" customWidth="1"/>
-    <col min="91" max="91" width="41.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="33.85546875" style="8" customWidth="1"/>
-    <col min="93" max="93" width="20.140625" style="8" customWidth="1"/>
-    <col min="94" max="94" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="31" style="8" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="27.140625" style="8" customWidth="1"/>
-    <col min="100" max="100" width="19.7109375" style="8" customWidth="1"/>
-    <col min="101" max="101" width="17.7109375" style="8" customWidth="1"/>
-    <col min="102" max="102" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="27" style="8" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="19.5703125" style="8" customWidth="1"/>
-    <col min="105" max="105" width="29.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="35.140625" style="8" customWidth="1"/>
-    <col min="107" max="107" width="31.85546875" style="8" customWidth="1"/>
-    <col min="108" max="108" width="20.7109375" style="8" customWidth="1"/>
-    <col min="109" max="109" width="31.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="19" style="8" customWidth="1"/>
-    <col min="111" max="111" width="23.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="20.7109375" style="8" customWidth="1"/>
-    <col min="113" max="113" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="27.28515625" style="8" customWidth="1"/>
-    <col min="115" max="115" width="23.28515625" style="8" customWidth="1"/>
-    <col min="116" max="116" width="24.42578125" style="8" customWidth="1"/>
-    <col min="117" max="117" width="16.28515625" style="8" customWidth="1"/>
-    <col min="118" max="118" width="51.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="27.28515625" style="8" customWidth="1"/>
-    <col min="120" max="120" width="23.28515625" style="8" customWidth="1"/>
-    <col min="121" max="121" width="24.42578125" style="8" customWidth="1"/>
-    <col min="122" max="122" width="16.28515625" style="8" customWidth="1"/>
-    <col min="123" max="123" width="20.7109375" style="8" customWidth="1"/>
-    <col min="124" max="124" width="63.5703125" style="8" customWidth="1"/>
-    <col min="125" max="125" width="30.85546875" style="8" customWidth="1"/>
-    <col min="126" max="126" width="27" style="8" customWidth="1"/>
-    <col min="127" max="127" width="23.28515625" style="8" customWidth="1"/>
-    <col min="128" max="128" width="44.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="33.5703125" style="8" customWidth="1"/>
-    <col min="130" max="131" width="20.7109375" style="8" customWidth="1"/>
-    <col min="132" max="132" width="63.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="30.85546875" style="8" customWidth="1"/>
-    <col min="134" max="134" width="27" style="8" customWidth="1"/>
-    <col min="135" max="135" width="23.28515625" style="8" customWidth="1"/>
-    <col min="136" max="136" width="44.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="33.5703125" style="8" customWidth="1"/>
-    <col min="138" max="138" width="28.42578125" style="8" customWidth="1"/>
-    <col min="139" max="139" width="27.7109375" style="8" customWidth="1"/>
-    <col min="140" max="140" width="43.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="36.7109375" style="8" customWidth="1"/>
-    <col min="142" max="142" width="29.140625" style="8" customWidth="1"/>
-    <col min="143" max="143" width="34" style="8" customWidth="1"/>
-    <col min="144" max="144" width="28.5703125" style="8" customWidth="1"/>
-    <col min="145" max="145" width="36.5703125" style="8" customWidth="1"/>
-    <col min="146" max="146" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="156" max="163" width="11.42578125" style="1"/>
-    <col min="164" max="165" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="168" max="173" width="11.42578125" style="1"/>
-    <col min="174" max="174" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="175" max="177" width="11.42578125" style="1"/>
-    <col min="178" max="178" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="11.42578125" style="1"/>
-    <col min="185" max="185" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="11.42578125" style="1"/>
-    <col min="187" max="187" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="11.42578125" style="1"/>
-    <col min="190" max="192" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="194" max="197" width="11.42578125" style="1"/>
-    <col min="198" max="198" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="199" max="202" width="11.42578125" style="1"/>
-    <col min="203" max="203" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="204" max="205" width="11.42578125" style="1"/>
-    <col min="206" max="207" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="211" max="213" width="11.42578125" style="1"/>
-    <col min="214" max="214" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="215" max="216" width="11.42578125" style="1"/>
-    <col min="217" max="217" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="221" max="223" width="11.42578125" style="1"/>
-    <col min="224" max="224" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="225" max="226" width="11.42578125" style="1"/>
-    <col min="227" max="228" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="232" max="234" width="11.42578125" style="1"/>
-    <col min="235" max="235" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="236" max="238" width="11.42578125" style="1"/>
-    <col min="239" max="239" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="240" max="242" width="11.42578125" style="1"/>
-    <col min="243" max="243" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="244" max="246" width="11.42578125" style="1"/>
-    <col min="247" max="247" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="251" max="253" width="11.42578125" style="1"/>
-    <col min="254" max="254" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="255" max="257" width="11.42578125" style="1"/>
-    <col min="258" max="258" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="259" max="261" width="11.42578125" style="1"/>
-    <col min="262" max="262" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="263" max="265" width="11.42578125" style="1"/>
-    <col min="266" max="266" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="267" max="268" width="11.42578125" style="1"/>
-    <col min="269" max="269" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="270" max="271" width="11.42578125" style="1"/>
-    <col min="272" max="272" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="273" max="274" width="11.42578125" style="1"/>
-    <col min="275" max="275" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="276" max="277" width="11.42578125" style="1"/>
-    <col min="278" max="278" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="279" max="280" width="11.42578125" style="1"/>
-    <col min="281" max="281" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="282" max="283" width="11.42578125" style="1"/>
-    <col min="284" max="284" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="286" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="21" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="25" style="3" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14" style="3" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27" style="3" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="36.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29" style="3" customWidth="1"/>
+    <col min="23" max="23" width="35.85546875" style="3" customWidth="1"/>
+    <col min="24" max="24" width="43.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="50.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="39.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="39.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.5703125" style="3" customWidth="1"/>
+    <col min="31" max="31" width="47.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="53.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="43" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="44.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="44.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="51.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="43.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="59" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="37.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="30.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="36.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="44.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="40.140625" style="3" customWidth="1"/>
+    <col min="49" max="49" width="40.28515625" style="3" customWidth="1"/>
+    <col min="50" max="50" width="34" style="3" customWidth="1"/>
+    <col min="51" max="51" width="40.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="47.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="39.140625" style="3" customWidth="1"/>
+    <col min="54" max="54" width="54.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="43.42578125" style="3" customWidth="1"/>
+    <col min="56" max="56" width="45.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="46.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="45.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="52.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="44" style="3" customWidth="1"/>
+    <col min="61" max="61" width="59.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.28515625" style="3" customWidth="1"/>
+    <col min="63" max="63" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="19.28515625" style="3" customWidth="1"/>
+    <col min="65" max="65" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20" style="3" customWidth="1"/>
+    <col min="67" max="67" width="35" style="3" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="28.42578125" style="3" customWidth="1"/>
+    <col min="69" max="69" width="23" style="3" customWidth="1"/>
+    <col min="70" max="70" width="17.7109375" style="3" customWidth="1"/>
+    <col min="71" max="71" width="24.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="29.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="21" style="3" customWidth="1"/>
+    <col min="75" max="75" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="29.42578125" style="3" customWidth="1"/>
+    <col min="77" max="77" width="21" style="3" customWidth="1"/>
+    <col min="78" max="78" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="29.42578125" style="3" customWidth="1"/>
+    <col min="80" max="80" width="21" style="3" customWidth="1"/>
+    <col min="81" max="81" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="29.42578125" style="3" customWidth="1"/>
+    <col min="83" max="83" width="21" style="3" customWidth="1"/>
+    <col min="84" max="84" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="29.42578125" style="3" customWidth="1"/>
+    <col min="86" max="86" width="21" style="3" customWidth="1"/>
+    <col min="87" max="87" width="31.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="19" style="3" customWidth="1"/>
+    <col min="89" max="89" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="30" style="3" customWidth="1"/>
+    <col min="91" max="91" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="33.85546875" style="3" customWidth="1"/>
+    <col min="93" max="93" width="20.140625" style="3" customWidth="1"/>
+    <col min="94" max="94" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="27.140625" style="3" customWidth="1"/>
+    <col min="100" max="100" width="19.7109375" style="3" customWidth="1"/>
+    <col min="101" max="101" width="17.7109375" style="3" customWidth="1"/>
+    <col min="102" max="102" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="27" style="3" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="19.5703125" style="3" customWidth="1"/>
+    <col min="105" max="105" width="29.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="35.140625" style="3" customWidth="1"/>
+    <col min="107" max="107" width="31.85546875" style="3" customWidth="1"/>
+    <col min="108" max="108" width="20.7109375" style="3" customWidth="1"/>
+    <col min="109" max="109" width="31.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="19" style="3" customWidth="1"/>
+    <col min="111" max="111" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="20.7109375" style="3" customWidth="1"/>
+    <col min="113" max="113" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="27.28515625" style="3" customWidth="1"/>
+    <col min="115" max="115" width="23.28515625" style="3" customWidth="1"/>
+    <col min="116" max="116" width="24.42578125" style="3" customWidth="1"/>
+    <col min="117" max="117" width="16.28515625" style="3" customWidth="1"/>
+    <col min="118" max="118" width="51.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="27.28515625" style="3" customWidth="1"/>
+    <col min="120" max="120" width="23.28515625" style="3" customWidth="1"/>
+    <col min="121" max="121" width="24.42578125" style="3" customWidth="1"/>
+    <col min="122" max="122" width="16.28515625" style="3" customWidth="1"/>
+    <col min="123" max="123" width="20.7109375" style="3" customWidth="1"/>
+    <col min="124" max="124" width="63.5703125" style="3" customWidth="1"/>
+    <col min="125" max="125" width="30.85546875" style="3" customWidth="1"/>
+    <col min="126" max="126" width="27" style="3" customWidth="1"/>
+    <col min="127" max="127" width="23.28515625" style="3" customWidth="1"/>
+    <col min="128" max="128" width="44.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="33.5703125" style="3" customWidth="1"/>
+    <col min="130" max="130" width="20.7109375" style="3" customWidth="1"/>
+    <col min="131" max="131" width="63.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="30.85546875" style="3" customWidth="1"/>
+    <col min="133" max="133" width="27" style="3" customWidth="1"/>
+    <col min="134" max="134" width="23.28515625" style="3" customWidth="1"/>
+    <col min="135" max="135" width="44.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="33.5703125" style="3" customWidth="1"/>
+    <col min="137" max="137" width="28.42578125" style="3" customWidth="1"/>
+    <col min="138" max="138" width="27.7109375" style="3" customWidth="1"/>
+    <col min="139" max="139" width="43.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="36.7109375" style="3" customWidth="1"/>
+    <col min="141" max="141" width="29.140625" style="3" customWidth="1"/>
+    <col min="142" max="142" width="34" style="3" customWidth="1"/>
+    <col min="143" max="143" width="28.5703125" style="3" customWidth="1"/>
+    <col min="144" max="144" width="36.5703125" style="3" customWidth="1"/>
+    <col min="145" max="145" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="155" max="162" width="11.42578125" style="1"/>
+    <col min="163" max="164" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="167" max="172" width="11.42578125" style="1"/>
+    <col min="173" max="173" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="174" max="176" width="11.42578125" style="1"/>
+    <col min="177" max="177" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="11.42578125" style="1"/>
+    <col min="184" max="184" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="11.42578125" style="1"/>
+    <col min="186" max="186" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="11.42578125" style="1"/>
+    <col min="189" max="191" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="193" max="196" width="11.42578125" style="1"/>
+    <col min="197" max="197" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="198" max="201" width="11.42578125" style="1"/>
+    <col min="202" max="202" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="203" max="204" width="11.42578125" style="1"/>
+    <col min="205" max="206" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="210" max="212" width="11.42578125" style="1"/>
+    <col min="213" max="213" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="214" max="215" width="11.42578125" style="1"/>
+    <col min="216" max="216" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="220" max="222" width="11.42578125" style="1"/>
+    <col min="223" max="223" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="224" max="225" width="11.42578125" style="1"/>
+    <col min="226" max="227" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="231" max="233" width="11.42578125" style="1"/>
+    <col min="234" max="234" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="235" max="237" width="11.42578125" style="1"/>
+    <col min="238" max="238" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="239" max="241" width="11.42578125" style="1"/>
+    <col min="242" max="242" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="243" max="245" width="11.42578125" style="1"/>
+    <col min="246" max="246" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="250" max="252" width="11.42578125" style="1"/>
+    <col min="253" max="253" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="254" max="256" width="11.42578125" style="1"/>
+    <col min="257" max="257" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="258" max="260" width="11.42578125" style="1"/>
+    <col min="261" max="261" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="262" max="264" width="11.42578125" style="1"/>
+    <col min="265" max="265" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="266" max="267" width="11.42578125" style="1"/>
+    <col min="268" max="268" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="269" max="270" width="11.42578125" style="1"/>
+    <col min="271" max="271" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="272" max="273" width="11.42578125" style="1"/>
+    <col min="274" max="274" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="275" max="276" width="11.42578125" style="1"/>
+    <col min="277" max="277" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="278" max="279" width="11.42578125" style="1"/>
+    <col min="280" max="280" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="282" width="11.42578125" style="1"/>
+    <col min="283" max="283" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="284" max="284" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="285" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:145" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:144" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>144</v>
       </c>
@@ -3662,16 +3649,15 @@
       <c r="EL1" s="1"/>
       <c r="EM1" s="1"/>
       <c r="EN1" s="1"/>
-      <c r="EO1" s="1"/>
     </row>
-    <row r="2" spans="1:145" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:144" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3811,9 +3797,8 @@
       <c r="EL2" s="1"/>
       <c r="EM2" s="1"/>
       <c r="EN2" s="1"/>
-      <c r="EO2" s="1"/>
     </row>
-    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:144" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -3958,9 +3943,8 @@
       <c r="EL3" s="1"/>
       <c r="EM3" s="1"/>
       <c r="EN3" s="1"/>
-      <c r="EO3" s="1"/>
     </row>
-    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:144" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4352,48 +4336,45 @@
         <v>133</v>
       </c>
       <c r="EA4" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="EB4" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="EC4" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="ED4" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="EE4" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="EF4" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="EG4" s="1" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="EH4" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="EI4" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="EJ4" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="EK4" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="EL4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="EM4" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="EN4" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="EO4" s="1" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>